<commit_message>
Badass File PMDM names (1).xlsx is freakin' committed.
</commit_message>
<xml_diff>
--- a/Mace/{path}/PMDM_Translated.xlsx
+++ b/Mace/{path}/PMDM_Translated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\AppData\Roaming\memsource\mso-converter\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD5CB936-192E-48FE-87A3-6A5F89663E7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26371189-116A-4977-9ECE-64EABDED7376}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1440" windowWidth="21060" windowHeight="10710"/>
+    <workbookView xWindow="960" yWindow="960" windowWidth="21060" windowHeight="10710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>